<commit_message>
Retrospectiva y registro de tiempos
Se creo la retrospectiva de la iteración pasada, se modifico la plantilla de tareas en algunos caso de uso, se registraron tiempos en las dos plantillas soibre los CU ya implementados y se creó la interfaz gráfica del CU-02 Editar renta
</commit_message>
<xml_diff>
--- a/Plantillas/Entrega 7/Plantilla Lista de Tareas de la Entrega 7.xlsx
+++ b/Plantillas/Entrega 7/Plantilla Lista de Tareas de la Entrega 7.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irdev\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irdev\OneDrive\Documentos\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01FC6B8D-FDCA-46E1-8DD0-1C81F9877CA2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC67DE80-96CE-4C0A-BAA6-8761ED83AAD9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="78">
   <si>
     <t>Columna</t>
   </si>
@@ -263,6 +263,9 @@
   </si>
   <si>
     <t>En este caso de uso el Maestro podrá dar de alta a un alumno a uno de sus grupos que tiene asignados</t>
+  </si>
+  <si>
+    <t>Hecho</t>
   </si>
 </sst>
 </file>
@@ -442,7 +445,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -565,6 +568,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -913,10 +919,10 @@
   <dimension ref="B1:BB57"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="AO44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A48" sqref="A48"/>
+      <selection pane="bottomRight" activeCell="BA49" sqref="BA48:BA49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5419,117 +5425,119 @@
       <c r="BA47" s="33"/>
       <c r="BB47" s="2"/>
     </row>
-    <row r="48" spans="2:54" s="39" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="40"/>
+    <row r="48" spans="2:54" s="39" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="34"/>
       <c r="C48" s="35"/>
-      <c r="D48" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="E48" s="34" t="s">
+      <c r="D48" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="E48" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="F48" s="40" t="s">
-        <v>45</v>
+      <c r="F48" s="37" t="s">
+        <v>53</v>
       </c>
       <c r="G48" s="41">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="H48" s="37"/>
       <c r="I48" s="37">
         <f t="shared" si="17"/>
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="J48" s="37"/>
       <c r="K48" s="37"/>
       <c r="L48" s="37">
-        <f t="shared" si="18"/>
-        <v>15</v>
+        <f>I48-K48</f>
+        <v>1</v>
       </c>
       <c r="M48" s="37"/>
       <c r="N48" s="37"/>
       <c r="O48" s="37">
-        <f t="shared" si="19"/>
-        <v>15</v>
+        <f>L48-N48</f>
+        <v>1</v>
       </c>
       <c r="P48" s="37"/>
-      <c r="Q48" s="37"/>
+      <c r="Q48" s="37">
+        <v>1</v>
+      </c>
       <c r="R48" s="37">
         <f t="shared" si="20"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="S48" s="37"/>
       <c r="T48" s="37"/>
       <c r="U48" s="37">
         <f t="shared" si="34"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="V48" s="37"/>
       <c r="W48" s="37"/>
       <c r="X48" s="37">
         <f t="shared" si="35"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="Y48" s="37"/>
       <c r="Z48" s="37"/>
       <c r="AA48" s="37">
         <f t="shared" si="23"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="AB48" s="37"/>
       <c r="AC48" s="37"/>
       <c r="AD48" s="37">
         <f t="shared" si="24"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="AE48" s="37"/>
       <c r="AF48" s="37"/>
       <c r="AG48" s="37">
         <f t="shared" si="25"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="AH48" s="37"/>
       <c r="AI48" s="37"/>
       <c r="AJ48" s="37">
         <f t="shared" si="26"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="AK48" s="37"/>
       <c r="AL48" s="37"/>
       <c r="AM48" s="37">
         <f t="shared" si="27"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="AN48" s="37"/>
       <c r="AO48" s="37"/>
       <c r="AP48" s="37">
         <f t="shared" si="28"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="AQ48" s="37"/>
       <c r="AR48" s="37"/>
       <c r="AS48" s="37">
         <f t="shared" si="29"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="AT48" s="37"/>
       <c r="AU48" s="37"/>
       <c r="AV48" s="37">
         <f t="shared" si="30"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="AW48" s="37"/>
       <c r="AX48" s="37"/>
       <c r="AY48" s="37">
         <f t="shared" si="31"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="AZ48" s="33">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA48" s="33">
         <f>G48-AZ48</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="BB48" s="2"/>
     </row>
@@ -5537,7 +5545,7 @@
       <c r="B49" s="40"/>
       <c r="C49" s="35"/>
       <c r="D49" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E49" s="34" t="s">
         <v>42</v>
@@ -5546,96 +5554,96 @@
         <v>45</v>
       </c>
       <c r="G49" s="41">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="H49" s="37"/>
       <c r="I49" s="37">
         <f t="shared" si="17"/>
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="J49" s="37"/>
       <c r="K49" s="37"/>
       <c r="L49" s="37">
-        <f t="shared" si="18"/>
-        <v>4</v>
+        <f>I49-K49</f>
+        <v>15</v>
       </c>
       <c r="M49" s="37"/>
       <c r="N49" s="37"/>
       <c r="O49" s="37">
-        <f t="shared" si="19"/>
-        <v>4</v>
+        <f>L49-N49</f>
+        <v>15</v>
       </c>
       <c r="P49" s="37"/>
       <c r="Q49" s="37"/>
       <c r="R49" s="37">
         <f t="shared" si="20"/>
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="S49" s="37"/>
       <c r="T49" s="37"/>
       <c r="U49" s="37">
         <f t="shared" si="34"/>
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="V49" s="37"/>
       <c r="W49" s="37"/>
       <c r="X49" s="37">
         <f t="shared" si="35"/>
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="Y49" s="37"/>
       <c r="Z49" s="37"/>
       <c r="AA49" s="37">
         <f t="shared" si="23"/>
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="AB49" s="37"/>
       <c r="AC49" s="37"/>
       <c r="AD49" s="37">
         <f t="shared" si="24"/>
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="AE49" s="37"/>
       <c r="AF49" s="37"/>
       <c r="AG49" s="37">
         <f t="shared" si="25"/>
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="AH49" s="37"/>
       <c r="AI49" s="37"/>
       <c r="AJ49" s="37">
         <f t="shared" si="26"/>
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="AK49" s="37"/>
       <c r="AL49" s="37"/>
       <c r="AM49" s="37">
         <f t="shared" si="27"/>
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="AN49" s="37"/>
       <c r="AO49" s="37"/>
       <c r="AP49" s="37">
         <f t="shared" si="28"/>
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="AQ49" s="37"/>
       <c r="AR49" s="37"/>
       <c r="AS49" s="37">
         <f t="shared" si="29"/>
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="AT49" s="37"/>
       <c r="AU49" s="37"/>
       <c r="AV49" s="37">
         <f t="shared" si="30"/>
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="AW49" s="37"/>
       <c r="AX49" s="37"/>
       <c r="AY49" s="37">
         <f t="shared" si="31"/>
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="AZ49" s="33">
         <f t="shared" si="32"/>
@@ -5643,581 +5651,587 @@
       </c>
       <c r="BA49" s="33">
         <f>G49-AZ49</f>
+        <v>15</v>
+      </c>
+      <c r="BB49" s="2"/>
+    </row>
+    <row r="50" spans="2:54" s="39" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="40"/>
+      <c r="C50" s="35"/>
+      <c r="D50" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="E50" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="F50" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="G50" s="41">
         <v>4</v>
       </c>
-      <c r="BB49" s="2"/>
-    </row>
-    <row r="50" spans="2:54" s="39" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="40" t="s">
-        <v>49</v>
-      </c>
-      <c r="C50" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="D50" s="34"/>
-      <c r="E50" s="34"/>
-      <c r="F50" s="37"/>
-      <c r="G50" s="41"/>
       <c r="H50" s="37"/>
-      <c r="I50" s="37"/>
+      <c r="I50" s="37">
+        <f t="shared" si="17"/>
+        <v>4</v>
+      </c>
       <c r="J50" s="37"/>
       <c r="K50" s="37"/>
-      <c r="L50" s="37"/>
+      <c r="L50" s="37">
+        <f t="shared" si="18"/>
+        <v>4</v>
+      </c>
       <c r="M50" s="37"/>
       <c r="N50" s="37"/>
-      <c r="O50" s="37"/>
+      <c r="O50" s="37">
+        <f t="shared" si="19"/>
+        <v>4</v>
+      </c>
       <c r="P50" s="37"/>
       <c r="Q50" s="37"/>
-      <c r="R50" s="37"/>
+      <c r="R50" s="37">
+        <f t="shared" si="20"/>
+        <v>4</v>
+      </c>
       <c r="S50" s="37"/>
       <c r="T50" s="37"/>
-      <c r="U50" s="37"/>
+      <c r="U50" s="37">
+        <f t="shared" si="34"/>
+        <v>4</v>
+      </c>
       <c r="V50" s="37"/>
       <c r="W50" s="37"/>
-      <c r="X50" s="37"/>
+      <c r="X50" s="37">
+        <f t="shared" si="35"/>
+        <v>4</v>
+      </c>
       <c r="Y50" s="37"/>
       <c r="Z50" s="37"/>
-      <c r="AA50" s="37"/>
+      <c r="AA50" s="37">
+        <f t="shared" si="23"/>
+        <v>4</v>
+      </c>
       <c r="AB50" s="37"/>
       <c r="AC50" s="37"/>
-      <c r="AD50" s="37"/>
+      <c r="AD50" s="37">
+        <f t="shared" si="24"/>
+        <v>4</v>
+      </c>
       <c r="AE50" s="37"/>
       <c r="AF50" s="37"/>
-      <c r="AG50" s="37"/>
+      <c r="AG50" s="37">
+        <f t="shared" si="25"/>
+        <v>4</v>
+      </c>
       <c r="AH50" s="37"/>
       <c r="AI50" s="37"/>
-      <c r="AJ50" s="37"/>
+      <c r="AJ50" s="37">
+        <f t="shared" si="26"/>
+        <v>4</v>
+      </c>
       <c r="AK50" s="37"/>
       <c r="AL50" s="37"/>
-      <c r="AM50" s="37"/>
+      <c r="AM50" s="37">
+        <f t="shared" si="27"/>
+        <v>4</v>
+      </c>
       <c r="AN50" s="37"/>
       <c r="AO50" s="37"/>
-      <c r="AP50" s="37"/>
+      <c r="AP50" s="37">
+        <f t="shared" si="28"/>
+        <v>4</v>
+      </c>
       <c r="AQ50" s="37"/>
       <c r="AR50" s="37"/>
-      <c r="AS50" s="37"/>
+      <c r="AS50" s="37">
+        <f t="shared" si="29"/>
+        <v>4</v>
+      </c>
       <c r="AT50" s="37"/>
       <c r="AU50" s="37"/>
-      <c r="AV50" s="37"/>
+      <c r="AV50" s="37">
+        <f t="shared" si="30"/>
+        <v>4</v>
+      </c>
       <c r="AW50" s="37"/>
       <c r="AX50" s="37"/>
-      <c r="AY50" s="37"/>
-      <c r="AZ50" s="33"/>
-      <c r="BA50" s="33"/>
+      <c r="AY50" s="37">
+        <f t="shared" si="31"/>
+        <v>4</v>
+      </c>
+      <c r="AZ50" s="33">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="BA50" s="33">
+        <f>G50-AZ50</f>
+        <v>4</v>
+      </c>
       <c r="BB50" s="2"/>
     </row>
-    <row r="51" spans="2:54" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="40"/>
-      <c r="C51" s="35"/>
-      <c r="D51" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="E51" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="F51" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="G51" s="41">
-        <v>5</v>
-      </c>
+    <row r="51" spans="2:54" s="39" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="C51" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="D51" s="34"/>
+      <c r="E51" s="34"/>
+      <c r="F51" s="37"/>
+      <c r="G51" s="41"/>
       <c r="H51" s="37"/>
-      <c r="I51" s="37">
-        <f t="shared" si="17"/>
-        <v>5</v>
-      </c>
+      <c r="I51" s="37"/>
       <c r="J51" s="37"/>
       <c r="K51" s="37"/>
-      <c r="L51" s="37">
-        <f t="shared" si="18"/>
-        <v>5</v>
-      </c>
+      <c r="L51" s="37"/>
       <c r="M51" s="37"/>
       <c r="N51" s="37"/>
-      <c r="O51" s="37">
-        <f t="shared" si="19"/>
-        <v>5</v>
-      </c>
+      <c r="O51" s="37"/>
       <c r="P51" s="37"/>
       <c r="Q51" s="37"/>
-      <c r="R51" s="37">
-        <f t="shared" si="20"/>
-        <v>5</v>
-      </c>
+      <c r="R51" s="37"/>
       <c r="S51" s="37"/>
       <c r="T51" s="37"/>
-      <c r="U51" s="37">
-        <f t="shared" si="34"/>
-        <v>5</v>
-      </c>
+      <c r="U51" s="37"/>
       <c r="V51" s="37"/>
       <c r="W51" s="37"/>
-      <c r="X51" s="37">
-        <f t="shared" si="35"/>
-        <v>5</v>
-      </c>
+      <c r="X51" s="37"/>
       <c r="Y51" s="37"/>
       <c r="Z51" s="37"/>
-      <c r="AA51" s="37">
-        <f t="shared" si="23"/>
-        <v>5</v>
-      </c>
+      <c r="AA51" s="37"/>
       <c r="AB51" s="37"/>
       <c r="AC51" s="37"/>
-      <c r="AD51" s="37">
-        <f t="shared" si="24"/>
-        <v>5</v>
-      </c>
+      <c r="AD51" s="37"/>
       <c r="AE51" s="37"/>
       <c r="AF51" s="37"/>
-      <c r="AG51" s="37">
-        <f t="shared" si="25"/>
-        <v>5</v>
-      </c>
+      <c r="AG51" s="37"/>
       <c r="AH51" s="37"/>
       <c r="AI51" s="37"/>
-      <c r="AJ51" s="37">
-        <f t="shared" si="26"/>
-        <v>5</v>
-      </c>
+      <c r="AJ51" s="37"/>
       <c r="AK51" s="37"/>
       <c r="AL51" s="37"/>
-      <c r="AM51" s="37">
-        <f t="shared" si="27"/>
-        <v>5</v>
-      </c>
+      <c r="AM51" s="37"/>
       <c r="AN51" s="37"/>
       <c r="AO51" s="37"/>
-      <c r="AP51" s="37">
-        <f t="shared" si="28"/>
-        <v>5</v>
-      </c>
+      <c r="AP51" s="37"/>
       <c r="AQ51" s="37"/>
       <c r="AR51" s="37"/>
-      <c r="AS51" s="37">
-        <f t="shared" si="29"/>
-        <v>5</v>
-      </c>
+      <c r="AS51" s="37"/>
       <c r="AT51" s="37"/>
       <c r="AU51" s="37"/>
-      <c r="AV51" s="37">
-        <f t="shared" si="30"/>
-        <v>5</v>
-      </c>
+      <c r="AV51" s="37"/>
       <c r="AW51" s="37"/>
       <c r="AX51" s="37"/>
-      <c r="AY51" s="37">
-        <f t="shared" si="31"/>
-        <v>5</v>
-      </c>
-      <c r="AZ51" s="33">
-        <f t="shared" si="32"/>
-        <v>0</v>
-      </c>
-      <c r="BA51" s="33">
-        <f t="shared" ref="BA51:BA56" si="40">G51-AZ51</f>
-        <v>5</v>
-      </c>
+      <c r="AY51" s="37"/>
+      <c r="AZ51" s="33"/>
+      <c r="BA51" s="33"/>
       <c r="BB51" s="2"/>
     </row>
     <row r="52" spans="2:54" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52" s="40"/>
       <c r="C52" s="35"/>
       <c r="D52" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E52" s="34" t="s">
         <v>42</v>
       </c>
       <c r="F52" s="37" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="G52" s="41">
-        <v>1</v>
-      </c>
-      <c r="H52" s="37"/>
+        <v>5</v>
+      </c>
+      <c r="H52" s="37">
+        <v>3</v>
+      </c>
       <c r="I52" s="37">
         <f t="shared" si="17"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J52" s="37"/>
       <c r="K52" s="37"/>
       <c r="L52" s="37">
         <f t="shared" si="18"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M52" s="37"/>
       <c r="N52" s="37"/>
       <c r="O52" s="37">
         <f t="shared" si="19"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P52" s="37"/>
       <c r="Q52" s="37"/>
       <c r="R52" s="37">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S52" s="37"/>
       <c r="T52" s="37"/>
       <c r="U52" s="37">
         <f t="shared" si="34"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V52" s="37"/>
       <c r="W52" s="37"/>
       <c r="X52" s="37">
         <f t="shared" si="35"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y52" s="37"/>
       <c r="Z52" s="37"/>
       <c r="AA52" s="37">
         <f t="shared" si="23"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB52" s="37"/>
       <c r="AC52" s="37"/>
       <c r="AD52" s="37">
         <f t="shared" si="24"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE52" s="37"/>
       <c r="AF52" s="37"/>
       <c r="AG52" s="37">
         <f t="shared" si="25"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH52" s="37"/>
       <c r="AI52" s="37"/>
       <c r="AJ52" s="37">
         <f t="shared" si="26"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK52" s="37"/>
       <c r="AL52" s="37"/>
       <c r="AM52" s="37">
         <f t="shared" si="27"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AN52" s="37"/>
       <c r="AO52" s="37"/>
       <c r="AP52" s="37">
         <f t="shared" si="28"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AQ52" s="37"/>
       <c r="AR52" s="37"/>
       <c r="AS52" s="37">
         <f t="shared" si="29"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AT52" s="37"/>
       <c r="AU52" s="37"/>
       <c r="AV52" s="37">
         <f t="shared" si="30"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AW52" s="37"/>
       <c r="AX52" s="37"/>
       <c r="AY52" s="37">
         <f t="shared" si="31"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AZ52" s="33">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BA52" s="33">
-        <f t="shared" si="40"/>
-        <v>1</v>
+        <f t="shared" ref="BA52:BA56" si="40">G52-AZ52</f>
+        <v>2</v>
       </c>
       <c r="BB52" s="2"/>
     </row>
-    <row r="53" spans="2:54" s="39" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="40" t="s">
-        <v>63</v>
-      </c>
-      <c r="C53" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="D53" s="34"/>
-      <c r="E53" s="34"/>
-      <c r="F53" s="37"/>
-      <c r="G53" s="41"/>
-      <c r="H53" s="37"/>
-      <c r="I53" s="37"/>
+    <row r="53" spans="2:54" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="40"/>
+      <c r="C53" s="35"/>
+      <c r="D53" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="E53" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="F53" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="G53" s="41">
+        <v>1</v>
+      </c>
+      <c r="H53" s="37">
+        <v>1</v>
+      </c>
+      <c r="I53" s="37">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
       <c r="J53" s="37"/>
       <c r="K53" s="37"/>
-      <c r="L53" s="37"/>
+      <c r="L53" s="37">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
       <c r="M53" s="37"/>
       <c r="N53" s="37"/>
-      <c r="O53" s="37"/>
+      <c r="O53" s="37">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
       <c r="P53" s="37"/>
       <c r="Q53" s="37"/>
-      <c r="R53" s="37"/>
+      <c r="R53" s="37">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
       <c r="S53" s="37"/>
       <c r="T53" s="37"/>
-      <c r="U53" s="37"/>
+      <c r="U53" s="37">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
       <c r="V53" s="37"/>
       <c r="W53" s="37"/>
-      <c r="X53" s="37"/>
+      <c r="X53" s="37">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
       <c r="Y53" s="37"/>
       <c r="Z53" s="37"/>
-      <c r="AA53" s="37"/>
+      <c r="AA53" s="37">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
       <c r="AB53" s="37"/>
       <c r="AC53" s="37"/>
-      <c r="AD53" s="37"/>
+      <c r="AD53" s="37">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
       <c r="AE53" s="37"/>
       <c r="AF53" s="37"/>
-      <c r="AG53" s="37"/>
+      <c r="AG53" s="37">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
       <c r="AH53" s="37"/>
       <c r="AI53" s="37"/>
-      <c r="AJ53" s="37"/>
+      <c r="AJ53" s="37">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
       <c r="AK53" s="37"/>
       <c r="AL53" s="37"/>
-      <c r="AM53" s="37"/>
+      <c r="AM53" s="37">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
       <c r="AN53" s="37"/>
       <c r="AO53" s="37"/>
-      <c r="AP53" s="37"/>
+      <c r="AP53" s="37">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
       <c r="AQ53" s="37"/>
       <c r="AR53" s="37"/>
-      <c r="AS53" s="37"/>
+      <c r="AS53" s="37">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
       <c r="AT53" s="37"/>
       <c r="AU53" s="37"/>
-      <c r="AV53" s="37"/>
+      <c r="AV53" s="37">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
       <c r="AW53" s="37"/>
       <c r="AX53" s="37"/>
-      <c r="AY53" s="37"/>
-      <c r="AZ53" s="33"/>
-      <c r="BA53" s="33"/>
+      <c r="AY53" s="37">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="AZ53" s="33">
+        <f t="shared" si="32"/>
+        <v>1</v>
+      </c>
+      <c r="BA53" s="33">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
       <c r="BB53" s="2"/>
     </row>
     <row r="54" spans="2:54" s="39" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="40"/>
-      <c r="C54" s="35"/>
-      <c r="D54" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="E54" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="F54" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="G54" s="41">
-        <v>2</v>
-      </c>
+      <c r="B54" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="C54" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="D54" s="34"/>
+      <c r="E54" s="34"/>
+      <c r="F54" s="37"/>
+      <c r="G54" s="41"/>
       <c r="H54" s="37"/>
-      <c r="I54" s="37">
-        <f t="shared" si="17"/>
-        <v>2</v>
-      </c>
+      <c r="I54" s="37"/>
       <c r="J54" s="37"/>
       <c r="K54" s="37"/>
-      <c r="L54" s="37">
-        <f t="shared" si="18"/>
-        <v>2</v>
-      </c>
+      <c r="L54" s="37"/>
       <c r="M54" s="37"/>
       <c r="N54" s="37"/>
-      <c r="O54" s="37">
-        <f t="shared" si="19"/>
-        <v>2</v>
-      </c>
+      <c r="O54" s="37"/>
       <c r="P54" s="37"/>
       <c r="Q54" s="37"/>
-      <c r="R54" s="37">
-        <f t="shared" si="20"/>
-        <v>2</v>
-      </c>
+      <c r="R54" s="37"/>
       <c r="S54" s="37"/>
       <c r="T54" s="37"/>
-      <c r="U54" s="37">
-        <f t="shared" si="34"/>
-        <v>2</v>
-      </c>
+      <c r="U54" s="37"/>
       <c r="V54" s="37"/>
       <c r="W54" s="37"/>
-      <c r="X54" s="37">
-        <f t="shared" si="35"/>
-        <v>2</v>
-      </c>
+      <c r="X54" s="37"/>
       <c r="Y54" s="37"/>
       <c r="Z54" s="37"/>
-      <c r="AA54" s="37">
-        <f t="shared" si="23"/>
-        <v>2</v>
-      </c>
+      <c r="AA54" s="37"/>
       <c r="AB54" s="37"/>
       <c r="AC54" s="37"/>
-      <c r="AD54" s="37">
-        <f t="shared" si="24"/>
-        <v>2</v>
-      </c>
+      <c r="AD54" s="37"/>
       <c r="AE54" s="37"/>
       <c r="AF54" s="37"/>
-      <c r="AG54" s="37">
-        <f t="shared" si="25"/>
-        <v>2</v>
-      </c>
+      <c r="AG54" s="37"/>
       <c r="AH54" s="37"/>
       <c r="AI54" s="37"/>
-      <c r="AJ54" s="37">
-        <f t="shared" si="26"/>
-        <v>2</v>
-      </c>
+      <c r="AJ54" s="37"/>
       <c r="AK54" s="37"/>
       <c r="AL54" s="37"/>
-      <c r="AM54" s="37">
-        <f t="shared" si="27"/>
-        <v>2</v>
-      </c>
+      <c r="AM54" s="37"/>
       <c r="AN54" s="37"/>
       <c r="AO54" s="37"/>
-      <c r="AP54" s="37">
-        <f t="shared" si="28"/>
-        <v>2</v>
-      </c>
+      <c r="AP54" s="37"/>
       <c r="AQ54" s="37"/>
       <c r="AR54" s="37"/>
-      <c r="AS54" s="37">
-        <f t="shared" si="29"/>
-        <v>2</v>
-      </c>
+      <c r="AS54" s="37"/>
       <c r="AT54" s="37"/>
       <c r="AU54" s="37"/>
-      <c r="AV54" s="37">
-        <f t="shared" si="30"/>
-        <v>2</v>
-      </c>
+      <c r="AV54" s="37"/>
       <c r="AW54" s="37"/>
       <c r="AX54" s="37"/>
-      <c r="AY54" s="37">
-        <f t="shared" si="31"/>
-        <v>2</v>
-      </c>
-      <c r="AZ54" s="33">
-        <f t="shared" si="32"/>
-        <v>0</v>
-      </c>
-      <c r="BA54" s="33">
-        <f t="shared" si="40"/>
-        <v>2</v>
-      </c>
+      <c r="AY54" s="37"/>
+      <c r="AZ54" s="33"/>
+      <c r="BA54" s="33"/>
       <c r="BB54" s="2"/>
     </row>
-    <row r="55" spans="2:54" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:54" s="39" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="40"/>
       <c r="C55" s="35"/>
       <c r="D55" s="34" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="E55" s="34" t="s">
         <v>42</v>
       </c>
       <c r="F55" s="37" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="G55" s="41">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H55" s="37"/>
       <c r="I55" s="37">
         <f t="shared" si="17"/>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="J55" s="37"/>
       <c r="K55" s="37"/>
       <c r="L55" s="37">
         <f t="shared" si="18"/>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="M55" s="37"/>
-      <c r="N55" s="37"/>
+      <c r="N55" s="37">
+        <v>1</v>
+      </c>
       <c r="O55" s="37">
         <f t="shared" si="19"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="P55" s="37"/>
       <c r="Q55" s="37"/>
       <c r="R55" s="37">
         <f t="shared" si="20"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="S55" s="37"/>
       <c r="T55" s="37"/>
       <c r="U55" s="37">
         <f t="shared" si="34"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="V55" s="37"/>
       <c r="W55" s="37"/>
       <c r="X55" s="37">
         <f t="shared" si="35"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="Y55" s="37"/>
       <c r="Z55" s="37"/>
       <c r="AA55" s="37">
         <f t="shared" si="23"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="AB55" s="37"/>
       <c r="AC55" s="37"/>
       <c r="AD55" s="37">
         <f t="shared" si="24"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="AE55" s="37"/>
       <c r="AF55" s="37"/>
       <c r="AG55" s="37">
         <f t="shared" si="25"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="AH55" s="37"/>
       <c r="AI55" s="37"/>
       <c r="AJ55" s="37">
         <f t="shared" si="26"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="AK55" s="37"/>
       <c r="AL55" s="37"/>
       <c r="AM55" s="37">
         <f t="shared" si="27"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="AN55" s="37"/>
       <c r="AO55" s="37"/>
       <c r="AP55" s="37">
         <f t="shared" si="28"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="AQ55" s="37"/>
       <c r="AR55" s="37"/>
       <c r="AS55" s="37">
         <f t="shared" si="29"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="AT55" s="37"/>
       <c r="AU55" s="37"/>
       <c r="AV55" s="37">
         <f t="shared" si="30"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="AW55" s="37"/>
       <c r="AX55" s="37"/>
       <c r="AY55" s="37">
         <f t="shared" si="31"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="AZ55" s="33">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA55" s="33">
         <f t="shared" si="40"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="BB55" s="2"/>
     </row>
@@ -6225,113 +6239,115 @@
       <c r="B56" s="40"/>
       <c r="C56" s="35"/>
       <c r="D56" s="34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E56" s="34" t="s">
         <v>42</v>
       </c>
       <c r="F56" s="37" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="G56" s="41">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H56" s="37"/>
       <c r="I56" s="37">
         <f t="shared" si="17"/>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="J56" s="37"/>
       <c r="K56" s="37"/>
       <c r="L56" s="37">
         <f t="shared" si="18"/>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="M56" s="37"/>
-      <c r="N56" s="37"/>
+      <c r="N56" s="37">
+        <v>4</v>
+      </c>
       <c r="O56" s="37">
         <f t="shared" si="19"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="P56" s="37"/>
       <c r="Q56" s="37"/>
       <c r="R56" s="37">
         <f t="shared" si="20"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="S56" s="37"/>
       <c r="T56" s="37"/>
       <c r="U56" s="37">
         <f t="shared" si="34"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="V56" s="37"/>
       <c r="W56" s="37"/>
       <c r="X56" s="37">
         <f t="shared" si="35"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="Y56" s="37"/>
       <c r="Z56" s="37"/>
       <c r="AA56" s="37">
         <f t="shared" si="23"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="AB56" s="37"/>
       <c r="AC56" s="37"/>
       <c r="AD56" s="37">
         <f t="shared" si="24"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="AE56" s="37"/>
       <c r="AF56" s="37"/>
       <c r="AG56" s="37">
         <f t="shared" si="25"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="AH56" s="37"/>
       <c r="AI56" s="37"/>
       <c r="AJ56" s="37">
         <f t="shared" si="26"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="AK56" s="37"/>
       <c r="AL56" s="37"/>
       <c r="AM56" s="37">
         <f t="shared" si="27"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="AN56" s="37"/>
       <c r="AO56" s="37"/>
       <c r="AP56" s="37">
         <f t="shared" si="28"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="AQ56" s="37"/>
       <c r="AR56" s="37"/>
       <c r="AS56" s="37">
         <f t="shared" si="29"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="AT56" s="37"/>
       <c r="AU56" s="37"/>
       <c r="AV56" s="37">
         <f t="shared" si="30"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="AW56" s="37"/>
       <c r="AX56" s="37"/>
       <c r="AY56" s="37">
         <f t="shared" si="31"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="AZ56" s="33">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BA56" s="33">
         <f t="shared" si="40"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="BB56" s="2"/>
     </row>

</xml_diff>

<commit_message>
Descripciones faltantes y diagramas
Se agregaron descripciones faltantes y diagramas de un CU
</commit_message>
<xml_diff>
--- a/Plantillas/Entrega 7/Plantilla Lista de Tareas de la Entrega 7.xlsx
+++ b/Plantillas/Entrega 7/Plantilla Lista de Tareas de la Entrega 7.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irdev\OneDrive\Documentos\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iro19\Documents\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC67DE80-96CE-4C0A-BAA6-8761ED83AAD9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6873F6-DE1E-437B-B502-8F29E78590A1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="79">
   <si>
     <t>Columna</t>
   </si>
@@ -266,6 +266,9 @@
   </si>
   <si>
     <t>Hecho</t>
+  </si>
+  <si>
+    <t>Descartado</t>
   </si>
 </sst>
 </file>
@@ -563,14 +566,14 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -919,10 +922,10 @@
   <dimension ref="B1:BB57"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="AO44" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="BA49" sqref="BA48:BA49"/>
+      <selection pane="bottomRight" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1004,84 +1007,84 @@
       <c r="BA3" s="2"/>
     </row>
     <row r="4" spans="2:54" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H4" s="47" t="s">
-        <v>5</v>
-      </c>
-      <c r="I4" s="48"/>
+      <c r="H4" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="49"/>
       <c r="J4" s="8"/>
-      <c r="K4" s="47" t="s">
+      <c r="K4" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="48"/>
+      <c r="L4" s="49"/>
       <c r="M4" s="8"/>
-      <c r="N4" s="47" t="s">
+      <c r="N4" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="48"/>
+      <c r="O4" s="49"/>
       <c r="P4" s="8"/>
-      <c r="Q4" s="47" t="s">
+      <c r="Q4" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="R4" s="48"/>
+      <c r="R4" s="49"/>
       <c r="S4" s="8"/>
-      <c r="T4" s="47" t="s">
+      <c r="T4" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="U4" s="48"/>
+      <c r="U4" s="49"/>
       <c r="V4" s="8"/>
-      <c r="W4" s="47" t="s">
+      <c r="W4" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="X4" s="48"/>
+      <c r="X4" s="49"/>
       <c r="Y4" s="8"/>
-      <c r="Z4" s="47" t="s">
+      <c r="Z4" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="AA4" s="48"/>
+      <c r="AA4" s="49"/>
       <c r="AB4" s="8"/>
-      <c r="AC4" s="47" t="s">
+      <c r="AC4" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="AD4" s="48"/>
+      <c r="AD4" s="49"/>
       <c r="AE4" s="8"/>
-      <c r="AF4" s="47" t="s">
+      <c r="AF4" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="AG4" s="48"/>
+      <c r="AG4" s="49"/>
       <c r="AH4" s="8"/>
-      <c r="AI4" s="47" t="s">
+      <c r="AI4" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="AJ4" s="48"/>
+      <c r="AJ4" s="49"/>
       <c r="AK4" s="8"/>
-      <c r="AL4" s="47" t="s">
+      <c r="AL4" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="AM4" s="48"/>
+      <c r="AM4" s="49"/>
       <c r="AN4" s="8"/>
-      <c r="AO4" s="47" t="s">
+      <c r="AO4" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="AP4" s="48"/>
+      <c r="AP4" s="49"/>
       <c r="AQ4" s="8"/>
-      <c r="AR4" s="47" t="s">
+      <c r="AR4" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="AS4" s="48"/>
+      <c r="AS4" s="49"/>
       <c r="AT4" s="8"/>
-      <c r="AU4" s="47" t="s">
+      <c r="AU4" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="AV4" s="48"/>
+      <c r="AV4" s="49"/>
       <c r="AW4" s="8"/>
-      <c r="AX4" s="47" t="s">
+      <c r="AX4" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="AY4" s="48"/>
-      <c r="AZ4" s="47" t="s">
+      <c r="AY4" s="49"/>
+      <c r="AZ4" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="BA4" s="48"/>
+      <c r="BA4" s="49"/>
     </row>
     <row r="5" spans="2:54" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
@@ -1282,7 +1285,7 @@
         <v>41</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="G7" s="24">
         <v>1</v>
@@ -1299,90 +1302,92 @@
         <v>1</v>
       </c>
       <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
+      <c r="N7" s="20">
+        <v>0.5</v>
+      </c>
       <c r="O7" s="20">
         <f t="shared" ref="O7:O9" si="2">L7-N7</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P7" s="20"/>
       <c r="Q7" s="20"/>
       <c r="R7" s="20">
         <f t="shared" ref="R7:R9" si="3">O7-Q7</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="S7" s="20"/>
       <c r="T7" s="20"/>
       <c r="U7" s="20">
         <f t="shared" ref="U7:U9" si="4">R7-T7</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="V7" s="20"/>
       <c r="W7" s="20"/>
       <c r="X7" s="20">
         <f t="shared" ref="X7:X9" si="5">U7-W7</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="Y7" s="20"/>
       <c r="Z7" s="20"/>
       <c r="AA7" s="20">
         <f t="shared" ref="AA7:AA9" si="6">X7-Z7</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AB7" s="20"/>
       <c r="AC7" s="20"/>
       <c r="AD7" s="20">
         <f t="shared" ref="AD7:AD9" si="7">AA7-AC7</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AE7" s="20"/>
       <c r="AF7" s="20"/>
       <c r="AG7" s="20">
         <f t="shared" ref="AG7:AG9" si="8">AD7-AF7</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AH7" s="20"/>
       <c r="AI7" s="20"/>
       <c r="AJ7" s="20">
         <f t="shared" ref="AJ7:AJ9" si="9">AG7-AI7</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AK7" s="20"/>
       <c r="AL7" s="20"/>
       <c r="AM7" s="20">
         <f t="shared" ref="AM7:AM9" si="10">AJ7-AL7</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AN7" s="20"/>
       <c r="AO7" s="20"/>
       <c r="AP7" s="20">
         <f t="shared" ref="AP7:AP9" si="11">AM7-AO7</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AQ7" s="20"/>
       <c r="AR7" s="20"/>
       <c r="AS7" s="20">
         <f t="shared" ref="AS7:AS9" si="12">AP7-AR7</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AT7" s="20"/>
       <c r="AU7" s="20"/>
       <c r="AV7" s="20">
         <f t="shared" ref="AV7:AV9" si="13">AS7-AU7</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AW7" s="20"/>
       <c r="AX7" s="20"/>
       <c r="AY7" s="20">
         <f t="shared" ref="AY7:AY9" si="14">AV7-AX7</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AZ7" s="33">
         <f t="shared" ref="AZ7:AZ9" si="15">H7+K7+N7+Q7+T7+W7+Z7+AC7+AF7+AI7+AL7+AO7+AR7+AU7+AX7</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="BA7" s="33">
         <f t="shared" ref="BA7:BA9" si="16">G7-AZ7</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="BB7" s="2"/>
     </row>
@@ -1396,7 +1401,7 @@
         <v>41</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="G8" s="24">
         <v>1</v>
@@ -1413,90 +1418,92 @@
         <v>1</v>
       </c>
       <c r="M8" s="20"/>
-      <c r="N8" s="20"/>
+      <c r="N8" s="20">
+        <v>0.5</v>
+      </c>
       <c r="O8" s="20">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P8" s="20"/>
       <c r="Q8" s="20"/>
       <c r="R8" s="20">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="S8" s="20"/>
       <c r="T8" s="20"/>
       <c r="U8" s="20">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="V8" s="20"/>
       <c r="W8" s="20"/>
       <c r="X8" s="20">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="Y8" s="20"/>
       <c r="Z8" s="20"/>
       <c r="AA8" s="20">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AB8" s="20"/>
       <c r="AC8" s="20"/>
       <c r="AD8" s="20">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AE8" s="20"/>
       <c r="AF8" s="20"/>
       <c r="AG8" s="20">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AH8" s="20"/>
       <c r="AI8" s="20"/>
       <c r="AJ8" s="20">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AK8" s="20"/>
       <c r="AL8" s="20"/>
       <c r="AM8" s="20">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AN8" s="20"/>
       <c r="AO8" s="20"/>
       <c r="AP8" s="20">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AQ8" s="20"/>
       <c r="AR8" s="20"/>
       <c r="AS8" s="20">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AT8" s="20"/>
       <c r="AU8" s="20"/>
       <c r="AV8" s="20">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AW8" s="20"/>
       <c r="AX8" s="20"/>
       <c r="AY8" s="20">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AZ8" s="33">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="BA8" s="33">
         <f t="shared" si="16"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="BB8" s="2"/>
     </row>
@@ -1794,7 +1801,7 @@
         <v>44</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="F12" s="17" t="s">
         <v>45</v>
@@ -1814,90 +1821,92 @@
         <v>1</v>
       </c>
       <c r="M12" s="20"/>
-      <c r="N12" s="20"/>
+      <c r="N12" s="20">
+        <v>1</v>
+      </c>
       <c r="O12" s="20">
         <f t="shared" si="19"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P12" s="20"/>
       <c r="Q12" s="20"/>
       <c r="R12" s="20">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S12" s="20"/>
       <c r="T12" s="20"/>
       <c r="U12" s="20">
         <f t="shared" ref="U12:U56" si="34">R12-T12</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V12" s="20"/>
       <c r="W12" s="20"/>
       <c r="X12" s="20">
         <f t="shared" ref="X12:X56" si="35">U12-W12</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y12" s="20"/>
       <c r="Z12" s="20"/>
       <c r="AA12" s="20">
         <f t="shared" si="23"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB12" s="20"/>
       <c r="AC12" s="20"/>
       <c r="AD12" s="20">
         <f t="shared" si="24"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE12" s="20"/>
       <c r="AF12" s="20"/>
       <c r="AG12" s="20">
         <f t="shared" si="25"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH12" s="20"/>
       <c r="AI12" s="20"/>
       <c r="AJ12" s="20">
         <f t="shared" si="26"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK12" s="20"/>
       <c r="AL12" s="20"/>
       <c r="AM12" s="20">
         <f t="shared" si="27"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN12" s="20"/>
       <c r="AO12" s="20"/>
       <c r="AP12" s="20">
         <f t="shared" si="28"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ12" s="20"/>
       <c r="AR12" s="20"/>
       <c r="AS12" s="20">
         <f t="shared" si="29"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT12" s="20"/>
       <c r="AU12" s="20"/>
       <c r="AV12" s="20">
         <f t="shared" si="30"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW12" s="20"/>
       <c r="AX12" s="20"/>
       <c r="AY12" s="20">
         <f t="shared" si="31"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ12" s="33">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA12" s="33">
         <f>G12-AZ12</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB12" s="2"/>
     </row>
@@ -1908,7 +1917,7 @@
         <v>43</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="F13" s="17" t="s">
         <v>45</v>
@@ -1928,90 +1937,92 @@
         <v>1</v>
       </c>
       <c r="M13" s="20"/>
-      <c r="N13" s="20"/>
+      <c r="N13" s="20">
+        <v>1</v>
+      </c>
       <c r="O13" s="20">
         <f t="shared" si="19"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P13" s="20"/>
       <c r="Q13" s="20"/>
       <c r="R13" s="20">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S13" s="20"/>
       <c r="T13" s="20"/>
       <c r="U13" s="20">
         <f t="shared" si="34"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V13" s="20"/>
       <c r="W13" s="20"/>
       <c r="X13" s="20">
         <f t="shared" si="35"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y13" s="20"/>
       <c r="Z13" s="20"/>
       <c r="AA13" s="20">
         <f t="shared" si="23"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB13" s="20"/>
       <c r="AC13" s="20"/>
       <c r="AD13" s="20">
         <f t="shared" si="24"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE13" s="20"/>
       <c r="AF13" s="20"/>
       <c r="AG13" s="20">
         <f t="shared" si="25"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH13" s="20"/>
       <c r="AI13" s="20"/>
       <c r="AJ13" s="20">
         <f t="shared" si="26"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK13" s="20"/>
       <c r="AL13" s="20"/>
       <c r="AM13" s="20">
         <f t="shared" si="27"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN13" s="20"/>
       <c r="AO13" s="20"/>
       <c r="AP13" s="20">
         <f t="shared" si="28"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ13" s="20"/>
       <c r="AR13" s="20"/>
       <c r="AS13" s="20">
         <f t="shared" si="29"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT13" s="20"/>
       <c r="AU13" s="20"/>
       <c r="AV13" s="20">
         <f t="shared" si="30"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW13" s="20"/>
       <c r="AX13" s="20"/>
       <c r="AY13" s="20">
         <f t="shared" si="31"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ13" s="33">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA13" s="33">
         <f>G13-AZ13</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB13" s="2"/>
     </row>
@@ -2423,7 +2434,7 @@
         <v>44</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="F18" s="17" t="s">
         <v>53</v>
@@ -2443,90 +2454,92 @@
         <v>1</v>
       </c>
       <c r="M18" s="20"/>
-      <c r="N18" s="20"/>
+      <c r="N18" s="20">
+        <v>1</v>
+      </c>
       <c r="O18" s="20">
         <f t="shared" si="19"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P18" s="20"/>
       <c r="Q18" s="20"/>
       <c r="R18" s="20">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S18" s="20"/>
       <c r="T18" s="20"/>
       <c r="U18" s="20">
         <f t="shared" si="34"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V18" s="20"/>
       <c r="W18" s="20"/>
       <c r="X18" s="20">
         <f t="shared" si="35"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y18" s="20"/>
       <c r="Z18" s="20"/>
       <c r="AA18" s="20">
         <f t="shared" si="23"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB18" s="20"/>
       <c r="AC18" s="20"/>
       <c r="AD18" s="20">
         <f t="shared" si="24"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE18" s="20"/>
       <c r="AF18" s="20"/>
       <c r="AG18" s="20">
         <f t="shared" si="25"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH18" s="20"/>
       <c r="AI18" s="20"/>
       <c r="AJ18" s="20">
         <f t="shared" si="26"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK18" s="20"/>
       <c r="AL18" s="20"/>
       <c r="AM18" s="20">
         <f t="shared" si="27"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN18" s="20"/>
       <c r="AO18" s="20"/>
       <c r="AP18" s="20">
         <f t="shared" si="28"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ18" s="20"/>
       <c r="AR18" s="20"/>
       <c r="AS18" s="20">
         <f t="shared" si="29"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT18" s="20"/>
       <c r="AU18" s="20"/>
       <c r="AV18" s="20">
         <f t="shared" si="30"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW18" s="20"/>
       <c r="AX18" s="20"/>
       <c r="AY18" s="20">
         <f t="shared" si="31"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ18" s="33">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA18" s="33">
         <f t="shared" si="36"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB18" s="2"/>
     </row>
@@ -2537,7 +2550,7 @@
         <v>43</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="F19" s="17" t="s">
         <v>53</v>
@@ -2557,90 +2570,92 @@
         <v>1</v>
       </c>
       <c r="M19" s="20"/>
-      <c r="N19" s="20"/>
+      <c r="N19" s="20">
+        <v>1</v>
+      </c>
       <c r="O19" s="20">
         <f t="shared" si="19"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P19" s="20"/>
       <c r="Q19" s="20"/>
       <c r="R19" s="20">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S19" s="20"/>
       <c r="T19" s="20"/>
       <c r="U19" s="20">
         <f t="shared" si="34"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V19" s="20"/>
       <c r="W19" s="20"/>
       <c r="X19" s="20">
         <f t="shared" si="35"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y19" s="20"/>
       <c r="Z19" s="20"/>
       <c r="AA19" s="20">
         <f t="shared" si="23"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB19" s="20"/>
       <c r="AC19" s="20"/>
       <c r="AD19" s="20">
         <f t="shared" si="24"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE19" s="20"/>
       <c r="AF19" s="20"/>
       <c r="AG19" s="20">
         <f t="shared" si="25"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH19" s="20"/>
       <c r="AI19" s="20"/>
       <c r="AJ19" s="20">
         <f t="shared" si="26"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK19" s="20"/>
       <c r="AL19" s="20"/>
       <c r="AM19" s="20">
         <f t="shared" si="27"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN19" s="20"/>
       <c r="AO19" s="20"/>
       <c r="AP19" s="20">
         <f t="shared" si="28"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ19" s="20"/>
       <c r="AR19" s="20"/>
       <c r="AS19" s="20">
         <f t="shared" si="29"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT19" s="20"/>
       <c r="AU19" s="20"/>
       <c r="AV19" s="20">
         <f t="shared" si="30"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW19" s="20"/>
       <c r="AX19" s="20"/>
       <c r="AY19" s="20">
         <f t="shared" si="31"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ19" s="33">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA19" s="33">
         <f t="shared" si="36"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB19" s="2"/>
     </row>
@@ -3055,7 +3070,7 @@
         <v>41</v>
       </c>
       <c r="F24" s="17" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="G24" s="24">
         <v>1</v>
@@ -3169,7 +3184,7 @@
         <v>41</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="G25" s="24">
         <v>1</v>
@@ -3283,7 +3298,7 @@
         <v>41</v>
       </c>
       <c r="F26" s="17" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="G26" s="24">
         <v>1</v>
@@ -3397,7 +3412,7 @@
         <v>41</v>
       </c>
       <c r="F27" s="17" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="G27" s="24">
         <v>5</v>
@@ -3511,7 +3526,7 @@
         <v>41</v>
       </c>
       <c r="F28" s="17" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="G28" s="24">
         <v>1</v>
@@ -5428,10 +5443,10 @@
     <row r="48" spans="2:54" s="39" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="34"/>
       <c r="C48" s="35"/>
-      <c r="D48" s="49" t="s">
+      <c r="D48" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="E48" s="49" t="s">
+      <c r="E48" s="47" t="s">
         <v>42</v>
       </c>
       <c r="F48" s="37" t="s">
@@ -6407,11 +6422,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -6423,6 +6433,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="50" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
Creación de interfaces gráficas
</commit_message>
<xml_diff>
--- a/Plantillas/Entrega 7/Plantilla Lista de Tareas de la Entrega 7.xlsx
+++ b/Plantillas/Entrega 7/Plantilla Lista de Tareas de la Entrega 7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iro19\Documents\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDDD36FB-A627-4F3F-8C7D-AF7050BD30F7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6554CE28-DCF1-4B48-8898-EF13132CC349}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -922,10 +922,10 @@
   <dimension ref="B1:BB57"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2036,7 +2036,7 @@
         <v>41</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="G14" s="24">
         <v>1</v>
@@ -2065,78 +2065,80 @@
         <v>1</v>
       </c>
       <c r="S14" s="20"/>
-      <c r="T14" s="20"/>
+      <c r="T14" s="20">
+        <v>2</v>
+      </c>
       <c r="U14" s="20">
         <f t="shared" si="34"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="V14" s="20"/>
       <c r="W14" s="20"/>
       <c r="X14" s="20">
         <f t="shared" si="35"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y14" s="20"/>
       <c r="Z14" s="20"/>
       <c r="AA14" s="20">
         <f t="shared" si="23"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AB14" s="20"/>
       <c r="AC14" s="20"/>
       <c r="AD14" s="20">
         <f t="shared" si="24"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AE14" s="20"/>
       <c r="AF14" s="20"/>
       <c r="AG14" s="20">
         <f t="shared" si="25"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AH14" s="20"/>
       <c r="AI14" s="20"/>
       <c r="AJ14" s="20">
         <f t="shared" si="26"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AK14" s="20"/>
       <c r="AL14" s="20"/>
       <c r="AM14" s="20">
         <f t="shared" si="27"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AN14" s="20"/>
       <c r="AO14" s="20"/>
       <c r="AP14" s="20">
         <f t="shared" si="28"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AQ14" s="20"/>
       <c r="AR14" s="20"/>
       <c r="AS14" s="20">
         <f t="shared" si="29"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AT14" s="20"/>
       <c r="AU14" s="20"/>
       <c r="AV14" s="20">
         <f t="shared" si="30"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AW14" s="20"/>
       <c r="AX14" s="20"/>
       <c r="AY14" s="20">
         <f t="shared" si="31"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AZ14" s="33">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA14" s="33">
         <f>G14-AZ14</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="BB14" s="2"/>
     </row>
@@ -2669,7 +2671,7 @@
         <v>41</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="G20" s="24">
         <v>1</v>
@@ -2698,78 +2700,80 @@
         <v>1</v>
       </c>
       <c r="S20" s="20"/>
-      <c r="T20" s="20"/>
+      <c r="T20" s="20">
+        <v>1</v>
+      </c>
       <c r="U20" s="20">
         <f t="shared" si="34"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V20" s="20"/>
       <c r="W20" s="20"/>
       <c r="X20" s="20">
         <f t="shared" si="35"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y20" s="20"/>
       <c r="Z20" s="20"/>
       <c r="AA20" s="20">
         <f t="shared" si="23"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB20" s="20"/>
       <c r="AC20" s="20"/>
       <c r="AD20" s="20">
         <f t="shared" si="24"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE20" s="20"/>
       <c r="AF20" s="20"/>
       <c r="AG20" s="20">
         <f t="shared" si="25"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH20" s="20"/>
       <c r="AI20" s="20"/>
       <c r="AJ20" s="20">
         <f t="shared" si="26"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK20" s="20"/>
       <c r="AL20" s="20"/>
       <c r="AM20" s="20">
         <f t="shared" si="27"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN20" s="20"/>
       <c r="AO20" s="20"/>
       <c r="AP20" s="20">
         <f t="shared" si="28"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ20" s="20"/>
       <c r="AR20" s="20"/>
       <c r="AS20" s="20">
         <f t="shared" si="29"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT20" s="20"/>
       <c r="AU20" s="20"/>
       <c r="AV20" s="20">
         <f t="shared" si="30"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW20" s="20"/>
       <c r="AX20" s="20"/>
       <c r="AY20" s="20">
         <f t="shared" si="31"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ20" s="33">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA20" s="33">
         <f t="shared" si="36"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB20" s="2"/>
     </row>
@@ -6422,11 +6426,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -6438,6 +6437,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="50" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
Pruebas unitarias y CU-18
Se realizó la implementación del CU 18 Registrar egresos variados y se realizarón las pruebas de este CU y del CU 17
</commit_message>
<xml_diff>
--- a/Plantillas/Entrega 7/Plantilla Lista de Tareas de la Entrega 7.xlsx
+++ b/Plantillas/Entrega 7/Plantilla Lista de Tareas de la Entrega 7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iro19\Documents\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19B880D-4A04-46FB-83A7-F04DA8CC2286}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E8849C-9E82-40FB-B39F-A9785F32B751}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -925,7 +925,7 @@
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2268,7 +2268,7 @@
         <v>41</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="G16" s="24">
         <v>1</v>
@@ -2309,66 +2309,68 @@
         <v>1</v>
       </c>
       <c r="Y16" s="20"/>
-      <c r="Z16" s="20"/>
+      <c r="Z16" s="20">
+        <v>1.5</v>
+      </c>
       <c r="AA16" s="20">
         <f t="shared" si="23"/>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="AB16" s="20"/>
       <c r="AC16" s="20"/>
       <c r="AD16" s="20">
         <f t="shared" si="24"/>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="AE16" s="20"/>
       <c r="AF16" s="20"/>
       <c r="AG16" s="20">
         <f t="shared" si="25"/>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="AH16" s="20"/>
       <c r="AI16" s="20"/>
       <c r="AJ16" s="20">
         <f t="shared" si="26"/>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="AK16" s="20"/>
       <c r="AL16" s="20"/>
       <c r="AM16" s="20">
         <f t="shared" si="27"/>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="AN16" s="20"/>
       <c r="AO16" s="20"/>
       <c r="AP16" s="20">
         <f t="shared" si="28"/>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="AQ16" s="20"/>
       <c r="AR16" s="20"/>
       <c r="AS16" s="20">
         <f t="shared" si="29"/>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="AT16" s="20"/>
       <c r="AU16" s="20"/>
       <c r="AV16" s="20">
         <f t="shared" si="30"/>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="AW16" s="20"/>
       <c r="AX16" s="20"/>
       <c r="AY16" s="20">
         <f t="shared" si="31"/>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="AZ16" s="33">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="BA16" s="33">
         <f t="shared" si="36"/>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="BB16" s="2"/>
     </row>
@@ -2789,7 +2791,7 @@
         <v>41</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="G21" s="24">
         <v>5</v>
@@ -2830,66 +2832,68 @@
         <v>5</v>
       </c>
       <c r="Y21" s="20"/>
-      <c r="Z21" s="20"/>
+      <c r="Z21" s="20">
+        <v>1</v>
+      </c>
       <c r="AA21" s="20">
         <f t="shared" si="23"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AB21" s="20"/>
       <c r="AC21" s="20"/>
       <c r="AD21" s="20">
         <f t="shared" si="24"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AE21" s="20"/>
       <c r="AF21" s="20"/>
       <c r="AG21" s="20">
         <f t="shared" si="25"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AH21" s="20"/>
       <c r="AI21" s="20"/>
       <c r="AJ21" s="20">
         <f t="shared" si="26"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AK21" s="20"/>
       <c r="AL21" s="20"/>
       <c r="AM21" s="20">
         <f t="shared" si="27"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AN21" s="20"/>
       <c r="AO21" s="20"/>
       <c r="AP21" s="20">
         <f t="shared" si="28"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AQ21" s="20"/>
       <c r="AR21" s="20"/>
       <c r="AS21" s="20">
         <f t="shared" si="29"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AT21" s="20"/>
       <c r="AU21" s="20"/>
       <c r="AV21" s="20">
         <f t="shared" si="30"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AW21" s="20"/>
       <c r="AX21" s="20"/>
       <c r="AY21" s="20">
         <f t="shared" si="31"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AZ21" s="33">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA21" s="33">
         <f t="shared" si="36"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BB21" s="2"/>
     </row>
@@ -2903,7 +2907,7 @@
         <v>41</v>
       </c>
       <c r="F22" s="17" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="G22" s="24">
         <v>1</v>
@@ -2944,66 +2948,68 @@
         <v>1</v>
       </c>
       <c r="Y22" s="20"/>
-      <c r="Z22" s="20"/>
+      <c r="Z22" s="20">
+        <v>0.5</v>
+      </c>
       <c r="AA22" s="20">
         <f t="shared" si="23"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AB22" s="20"/>
       <c r="AC22" s="20"/>
       <c r="AD22" s="20">
         <f t="shared" si="24"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AE22" s="20"/>
       <c r="AF22" s="20"/>
       <c r="AG22" s="20">
         <f t="shared" si="25"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AH22" s="20"/>
       <c r="AI22" s="20"/>
       <c r="AJ22" s="20">
         <f t="shared" si="26"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AK22" s="20"/>
       <c r="AL22" s="20"/>
       <c r="AM22" s="20">
         <f t="shared" si="27"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AN22" s="20"/>
       <c r="AO22" s="20"/>
       <c r="AP22" s="20">
         <f t="shared" si="28"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AQ22" s="20"/>
       <c r="AR22" s="20"/>
       <c r="AS22" s="20">
         <f t="shared" si="29"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AT22" s="20"/>
       <c r="AU22" s="20"/>
       <c r="AV22" s="20">
         <f t="shared" si="30"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AW22" s="20"/>
       <c r="AX22" s="20"/>
       <c r="AY22" s="20">
         <f t="shared" si="31"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AZ22" s="33">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="BA22" s="33">
         <f t="shared" si="36"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="BB22" s="2"/>
     </row>

</xml_diff>

<commit_message>
Implementación de CU 09 y correcciones
Se implementó el CU 09 y además se realizarón correcciones con respecto al momento de buscar alumnos, maestros o clientes
</commit_message>
<xml_diff>
--- a/Plantillas/Entrega 7/Plantilla Lista de Tareas de la Entrega 7.xlsx
+++ b/Plantillas/Entrega 7/Plantilla Lista de Tareas de la Entrega 7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iro19\Documents\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E8849C-9E82-40FB-B39F-A9785F32B751}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C626E12-3A9C-4940-B667-F43A8B1168C2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -448,7 +448,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -568,6 +568,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -925,7 +928,7 @@
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1007,84 +1010,84 @@
       <c r="BA3" s="2"/>
     </row>
     <row r="4" spans="2:54" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H4" s="48" t="s">
-        <v>5</v>
-      </c>
-      <c r="I4" s="49"/>
+      <c r="H4" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="50"/>
       <c r="J4" s="8"/>
-      <c r="K4" s="48" t="s">
+      <c r="K4" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="49"/>
+      <c r="L4" s="50"/>
       <c r="M4" s="8"/>
-      <c r="N4" s="48" t="s">
+      <c r="N4" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="49"/>
+      <c r="O4" s="50"/>
       <c r="P4" s="8"/>
-      <c r="Q4" s="48" t="s">
+      <c r="Q4" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="R4" s="49"/>
+      <c r="R4" s="50"/>
       <c r="S4" s="8"/>
-      <c r="T4" s="48" t="s">
+      <c r="T4" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="U4" s="49"/>
+      <c r="U4" s="50"/>
       <c r="V4" s="8"/>
-      <c r="W4" s="48" t="s">
+      <c r="W4" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="X4" s="49"/>
+      <c r="X4" s="50"/>
       <c r="Y4" s="8"/>
-      <c r="Z4" s="48" t="s">
+      <c r="Z4" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="AA4" s="49"/>
+      <c r="AA4" s="50"/>
       <c r="AB4" s="8"/>
-      <c r="AC4" s="48" t="s">
+      <c r="AC4" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="AD4" s="49"/>
+      <c r="AD4" s="50"/>
       <c r="AE4" s="8"/>
-      <c r="AF4" s="48" t="s">
+      <c r="AF4" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="AG4" s="49"/>
+      <c r="AG4" s="50"/>
       <c r="AH4" s="8"/>
-      <c r="AI4" s="48" t="s">
+      <c r="AI4" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="AJ4" s="49"/>
+      <c r="AJ4" s="50"/>
       <c r="AK4" s="8"/>
-      <c r="AL4" s="48" t="s">
+      <c r="AL4" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="AM4" s="49"/>
+      <c r="AM4" s="50"/>
       <c r="AN4" s="8"/>
-      <c r="AO4" s="48" t="s">
+      <c r="AO4" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="AP4" s="49"/>
+      <c r="AP4" s="50"/>
       <c r="AQ4" s="8"/>
-      <c r="AR4" s="48" t="s">
+      <c r="AR4" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="AS4" s="49"/>
+      <c r="AS4" s="50"/>
       <c r="AT4" s="8"/>
-      <c r="AU4" s="48" t="s">
+      <c r="AU4" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="AV4" s="49"/>
+      <c r="AV4" s="50"/>
       <c r="AW4" s="8"/>
-      <c r="AX4" s="48" t="s">
+      <c r="AX4" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="AY4" s="49"/>
-      <c r="AZ4" s="48" t="s">
+      <c r="AY4" s="50"/>
+      <c r="AZ4" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="BA4" s="49"/>
+      <c r="BA4" s="50"/>
     </row>
     <row r="5" spans="2:54" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
@@ -1517,7 +1520,7 @@
         <v>41</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="G9" s="24">
         <v>5</v>
@@ -1564,60 +1567,62 @@
         <v>5</v>
       </c>
       <c r="AB9" s="20"/>
-      <c r="AC9" s="20"/>
+      <c r="AC9" s="20">
+        <v>3</v>
+      </c>
       <c r="AD9" s="20">
         <f t="shared" si="7"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AE9" s="20"/>
       <c r="AF9" s="20"/>
       <c r="AG9" s="20">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AH9" s="20"/>
       <c r="AI9" s="20"/>
       <c r="AJ9" s="20">
         <f t="shared" si="9"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AK9" s="20"/>
       <c r="AL9" s="20"/>
       <c r="AM9" s="20">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AN9" s="20"/>
       <c r="AO9" s="20"/>
       <c r="AP9" s="20">
         <f t="shared" si="11"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AQ9" s="20"/>
       <c r="AR9" s="20"/>
       <c r="AS9" s="20">
         <f t="shared" si="12"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AT9" s="20"/>
       <c r="AU9" s="20"/>
       <c r="AV9" s="20">
         <f t="shared" si="13"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AW9" s="20"/>
       <c r="AX9" s="20"/>
       <c r="AY9" s="20">
         <f t="shared" si="14"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AZ9" s="33">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BA9" s="33">
         <f t="shared" si="16"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="BB9" s="2"/>
     </row>
@@ -1631,7 +1636,7 @@
         <v>41</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="G10" s="24">
         <v>2</v>
@@ -1678,60 +1683,62 @@
         <v>2</v>
       </c>
       <c r="AB10" s="20"/>
-      <c r="AC10" s="20"/>
+      <c r="AC10" s="20">
+        <v>1</v>
+      </c>
       <c r="AD10" s="20">
         <f t="shared" ref="AD10:AD56" si="24">AA10-AC10</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE10" s="20"/>
       <c r="AF10" s="20"/>
       <c r="AG10" s="20">
         <f t="shared" ref="AG10:AG56" si="25">AD10-AF10</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH10" s="20"/>
       <c r="AI10" s="20"/>
       <c r="AJ10" s="20">
         <f t="shared" ref="AJ10:AJ56" si="26">AG10-AI10</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK10" s="20"/>
       <c r="AL10" s="20"/>
       <c r="AM10" s="20">
         <f t="shared" ref="AM10:AM56" si="27">AJ10-AL10</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AN10" s="20"/>
       <c r="AO10" s="20"/>
       <c r="AP10" s="20">
         <f t="shared" ref="AP10:AP56" si="28">AM10-AO10</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AQ10" s="20"/>
       <c r="AR10" s="20"/>
       <c r="AS10" s="20">
         <f t="shared" ref="AS10:AS56" si="29">AP10-AR10</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AT10" s="20"/>
       <c r="AU10" s="20"/>
       <c r="AV10" s="20">
         <f t="shared" ref="AV10:AV56" si="30">AS10-AU10</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AW10" s="20"/>
       <c r="AX10" s="20"/>
       <c r="AY10" s="20">
         <f t="shared" ref="AY10:AY56" si="31">AV10-AX10</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AZ10" s="33">
         <f t="shared" ref="AZ10:AZ56" si="32">H10+K10+N10+Q10+T10+W10+Z10+AC10+AF10+AI10+AL10+AO10+AR10+AU10+AX10</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA10" s="33">
         <f t="shared" ref="BA10" si="33">G10-AZ10</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BB10" s="2"/>
     </row>
@@ -1801,7 +1808,7 @@
         <v>44</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="F12" s="17" t="s">
         <v>77</v>
@@ -1917,7 +1924,7 @@
         <v>43</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="F13" s="17" t="s">
         <v>77</v>
@@ -2440,7 +2447,7 @@
         <v>44</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="F18" s="17" t="s">
         <v>77</v>
@@ -2556,7 +2563,7 @@
         <v>43</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="F19" s="17" t="s">
         <v>77</v>
@@ -2671,7 +2678,7 @@
       <c r="D20" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="E20" s="23" t="s">
+      <c r="E20" s="48" t="s">
         <v>41</v>
       </c>
       <c r="F20" s="17" t="s">

</xml_diff>